<commit_message>
Modificaciones hasta tercera semana septiembre 23
</commit_message>
<xml_diff>
--- a/dags/files_pami/TerapiasDomi.xlsx
+++ b/dags/files_pami/TerapiasDomi.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26914"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clinicossasips-my.sharepoint.com/personal/maristizabal_clinicos_com_co/Documents/GESTIÓN DE TABLEROS/ACTUALIZACION PAMI Y CARTAGENA/DOMI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clinicos\OneDrive - CLINICOS PROGRAMAS DE ATENCION INTEGRAL SAS IPS\GESTIÓN DE TABLEROS\ACTUALIZACION PAMI Y CARTAGENA\DOMI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="164" documentId="8_{6B972476-2650-45EB-834C-459E3BBF69A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59B51E5F-87B7-4593-97D4-3341F7656E60}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E3DB03-8646-48C6-B439-E1CA1C2991A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{92DDBD9F-D42D-431C-8C8F-AA85B0C9E8F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -63,7 +63,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -483,12 +483,12 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,7 +499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="4">
         <v>45139</v>
       </c>
@@ -510,7 +510,7 @@
         <v>1542</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="4">
         <v>45139</v>
       </c>
@@ -518,10 +518,10 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>836</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="4">
         <v>45139</v>
       </c>
@@ -529,10 +529,10 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>1865</v>
+        <v>364</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="4">
         <v>45139</v>
       </c>
@@ -540,7 +540,7 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>869</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -549,6 +549,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E8AAD53D957193499A95B0822EE92604" ma:contentTypeVersion="5" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="64521337f70ab7452aeeac0760611e10">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b848449e-c9d3-4969-a575-ff0d96471e4b" xmlns:ns3="ac8deb47-86bc-4260-8fcd-a6158e6e95f4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bab967c49d094239a50a0e5887e9ad5e" ns2:_="" ns3:_="">
     <xsd:import namespace="b848449e-c9d3-4969-a575-ff0d96471e4b"/>
@@ -719,19 +728,20 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9B1E666-A035-4395-9FCE-7B0DF4122DCE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F91A3489-C7E9-4026-9E26-46E3D2077E1C}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47AA40F3-EB79-4A3D-88A0-542F91DDE506}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2C100DA-CAE7-431C-9519-D467025688B5}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E48649F2-B20F-4E4B-8137-C051F6519A2E}"/>
 </file>
</xml_diff>